<commit_message>
soting issue fixed in metadata
</commit_message>
<xml_diff>
--- a/MappingSheet/MapptingSheet_MySQL.xlsx
+++ b/MappingSheet/MapptingSheet_MySQL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bibhu\Workspace1\ETLAutomationProject4\MappingSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bibhu\etl-test-automation\MappingSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A0B10F-BF4E-42E7-9D63-6F5CC4B6B3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3C7EEE-C77C-4AF4-9B52-CA85811F6512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{79CB5CD8-2CCE-42B4-AB41-F9764ADA8C90}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{79CB5CD8-2CCE-42B4-AB41-F9764ADA8C90}"/>
   </bookViews>
   <sheets>
     <sheet name="T_EMP" sheetId="1" r:id="rId1"/>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DDDADE-0E00-49F1-8646-4DB74175C9F6}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BEFA2F4-0555-4A44-AD7F-2227EB459093}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
error message fixed for metadata testcase
</commit_message>
<xml_diff>
--- a/MappingSheet/MapptingSheet_MySQL.xlsx
+++ b/MappingSheet/MapptingSheet_MySQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bibhu\etl-test-automation\MappingSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3C7EEE-C77C-4AF4-9B52-CA85811F6512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C2592B-33D1-45C7-9406-F85A49D37A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{79CB5CD8-2CCE-42B4-AB41-F9764ADA8C90}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{79CB5CD8-2CCE-42B4-AB41-F9764ADA8C90}"/>
   </bookViews>
   <sheets>
     <sheet name="T_EMP" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>T_EMP</t>
   </si>
   <si>
-    <t>T_EMP_ID</t>
-  </si>
-  <si>
     <t>EMP_ID</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>VARCHAR2</t>
+  </si>
+  <si>
+    <t>T_EMP_ID</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,286 +743,286 @@
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -1034,22 +1034,22 @@
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -1061,16 +1061,16 @@
         <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -1148,94 +1148,94 @@
         <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I5" s="4"/>
     </row>

</xml_diff>

<commit_message>
updated log and error mechanism
</commit_message>
<xml_diff>
--- a/MappingSheet/MapptingSheet_MySQL.xlsx
+++ b/MappingSheet/MapptingSheet_MySQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bibhu\etl-test-automation\MappingSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C2592B-33D1-45C7-9406-F85A49D37A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C58461-D1CE-456E-856D-41830AB771E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{79CB5CD8-2CCE-42B4-AB41-F9764ADA8C90}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{79CB5CD8-2CCE-42B4-AB41-F9764ADA8C90}"/>
   </bookViews>
   <sheets>
     <sheet name="T_EMP" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>T_EMP</t>
   </si>
   <si>
-    <t>EMP_ID</t>
-  </si>
-  <si>
     <t>EMP_NAME</t>
   </si>
   <si>
@@ -272,7 +269,10 @@
     <t>VARCHAR2</t>
   </si>
   <si>
-    <t>T_EMP_ID</t>
+    <t>T_EMP_ID1212</t>
+  </si>
+  <si>
+    <t>EMP_ID345</t>
   </si>
 </sst>
 </file>
@@ -678,7 +678,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,286 +743,286 @@
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -1034,22 +1034,22 @@
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -1061,16 +1061,16 @@
         <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -1148,94 +1148,94 @@
         <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" s="4"/>
     </row>

</xml_diff>